<commit_message>
Formato de las variables modificado
</commit_message>
<xml_diff>
--- a/Datos/PH.xlsx
+++ b/Datos/PH.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,41 +448,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>12/05/25</t>
+          <t>05/01/25</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>13/05/25</t>
+          <t>06/01/25</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>14/05/25</t>
+          <t>07/01/25</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>15/05/25</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>8</v>
+        <v>2.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(Add): Agregamos la opción numero 2, para generar graficos de lineas y guardados de archivos
</commit_message>
<xml_diff>
--- a/Datos/PH.xlsx
+++ b/Datos/PH.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,16 @@
         <v>2.6</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>08/01/25</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>